<commit_message>
progress before meeting and figure 1
</commit_message>
<xml_diff>
--- a/data/idea_meeting_log.xlsx
+++ b/data/idea_meeting_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Spyrison\Documents\R\melb_datathon2020\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9678FFC6-7472-46FA-9910-1D3915A7DA5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0EEF1F-73FC-4ED1-8825-4FA945E327E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{9A74CA55-049F-425A-940E-63D6993ABE0C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11628" xr2:uid="{9A74CA55-049F-425A-940E-63D6993ABE0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ideas</t>
   </si>
@@ -99,13 +99,40 @@
     <t>Madeline, weather from</t>
   </si>
   <si>
-    <t>Madeline, gunction measurments</t>
-  </si>
-  <si>
     <t>Yang animating weekly aggregates against single lagged week above heatmap of daily usage</t>
   </si>
   <si>
     <t>pic</t>
+  </si>
+  <si>
+    <t>Madeline, fig 2 regresssions of agg Aug data</t>
+  </si>
+  <si>
+    <t>trend looks more yearly, rather than a jump in 2020</t>
+  </si>
+  <si>
+    <t>Yang, Matlab splines</t>
+  </si>
+  <si>
+    <t>Nick, R splines</t>
+  </si>
+  <si>
+    <t>fit splines in matlab, "not much diff than Madeline"</t>
+  </si>
+  <si>
+    <t>Madeline, function measurments</t>
+  </si>
+  <si>
+    <t>fit splines in r,working on roots, to get function measures.</t>
+  </si>
+  <si>
+    <t>Madeline, differing feature is trend with past trends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick, what about weekend, or weekend </t>
+  </si>
+  <si>
+    <t>This week's theme: Improve on last weeks ideas.</t>
   </si>
 </sst>
 </file>
@@ -528,24 +555,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85F12BC-4AF4-4562-8765-2DD7DB841DA7}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+    <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -571,18 +598,18 @@
         <v>44099</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4">
         <v>44099</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -592,7 +619,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -606,7 +633,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -618,7 +645,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -632,7 +659,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -643,7 +670,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -654,7 +681,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -665,7 +692,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -676,9 +703,48 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>